<commit_message>
add kpi analysis and correct source income file
</commit_message>
<xml_diff>
--- a/temporal_landing/2020_income.xlsx
+++ b/temporal_landing/2020_income.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Zhengyong Ji\Documents\GitHub\MDS-ADSDB-Proj1-JiJonas\temporal_landing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06171041-0F57-44E3-BDBD-5CFE84AAAEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65B77B3-AD1E-41E3-92F9-E7026E8CF224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{E1018A7A-359B-4CFD-A896-C78758860A03}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{E1018A7A-359B-4CFD-A896-C78758860A03}"/>
   </bookViews>
   <sheets>
     <sheet name="renda" sheetId="1" r:id="rId1"/>
@@ -917,13 +917,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{953D53C2-8B7F-4B57-9F33-EFAAF808FCBB}">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>158</v>
       </c>
@@ -943,1478 +943,1478 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>159</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2">
-        <v>11.178000000000001</v>
+      <c r="C2">
+        <v>11178</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2">
-        <v>11.999000000000001</v>
+      <c r="E2">
+        <v>11999</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>159</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2">
-        <v>15.99</v>
+      <c r="C3">
+        <v>15990</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2">
-        <v>18.667999999999999</v>
+      <c r="E3">
+        <v>18668</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>159</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2">
-        <v>13.246</v>
+      <c r="C4">
+        <v>13246</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="2">
-        <v>14.805999999999999</v>
+      <c r="E4">
+        <v>14806</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>159</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="2">
-        <v>16.77</v>
+      <c r="C5">
+        <v>16770</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="2">
-        <v>21.791</v>
+      <c r="E5">
+        <v>21791</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>160</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="2">
-        <v>21.045000000000002</v>
+      <c r="C6">
+        <v>21045</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="2">
-        <v>23.503</v>
+      <c r="E6">
+        <v>23503</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>160</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="2">
-        <v>17.116</v>
+      <c r="C7">
+        <v>17116</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="2">
-        <v>19.792999999999999</v>
+      <c r="E7">
+        <v>19793</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>160</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C8" s="2">
-        <v>27.942</v>
+      <c r="C8">
+        <v>27942</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="2">
-        <v>31.494</v>
+      <c r="E8">
+        <v>31494</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>160</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C9" s="2">
-        <v>24.765999999999998</v>
+      <c r="C9">
+        <v>24766</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="2">
-        <v>29.032</v>
+      <c r="E9">
+        <v>29032</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>160</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C10" s="2">
-        <v>23.393999999999998</v>
+      <c r="C10">
+        <v>23394</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="2">
-        <v>26.055</v>
+      <c r="E10">
+        <v>26055</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>160</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="2">
-        <v>22.927</v>
+      <c r="C11">
+        <v>22927</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="2">
-        <v>25.49</v>
+      <c r="E11">
+        <v>25490</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>161</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C12" s="2">
-        <v>16.391999999999999</v>
+      <c r="C12">
+        <v>16392</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="2">
-        <v>18.821999999999999</v>
+      <c r="E12">
+        <v>18822</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>161</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="C13" s="2">
-        <v>13.231999999999999</v>
+      <c r="C13">
+        <v>13232</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="2">
-        <v>16.282</v>
+      <c r="E13">
+        <v>16282</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>161</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="2">
-        <v>15.374000000000001</v>
+      <c r="C14">
+        <v>15374</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E14" s="2">
-        <v>17.681999999999999</v>
+      <c r="E14">
+        <v>17682</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>161</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="2">
-        <v>19.137</v>
+      <c r="C15">
+        <v>19137</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="2">
-        <v>19.969000000000001</v>
+      <c r="E15">
+        <v>19969</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>161</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="2">
-        <v>18.306999999999999</v>
+      <c r="C16">
+        <v>18307</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="2">
-        <v>20.332000000000001</v>
+      <c r="E16">
+        <v>20332</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>161</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="2">
-        <v>18.693000000000001</v>
+      <c r="C17">
+        <v>18693</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E17" s="2">
-        <v>21.591999999999999</v>
+      <c r="E17">
+        <v>21592</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>161</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C18" s="2">
-        <v>18.062999999999999</v>
+      <c r="C18">
+        <v>18063</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="2">
-        <v>18.843</v>
+      <c r="E18">
+        <v>18843</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>161</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="2">
-        <v>20.347999999999999</v>
+      <c r="C19">
+        <v>20348</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="2">
-        <v>22.843</v>
+      <c r="E19">
+        <v>22843</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>162</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="2">
-        <v>27.702000000000002</v>
+      <c r="C20">
+        <v>27702</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="2">
-        <v>30.198</v>
+      <c r="E20">
+        <v>30198</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>162</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="2">
-        <v>21.312999999999999</v>
+      <c r="C21">
+        <v>21313</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E21" s="2">
-        <v>25.029</v>
+      <c r="E21">
+        <v>25029</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>162</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="2">
-        <v>43.27</v>
+      <c r="C22">
+        <v>43270</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="2">
-        <v>56.466000000000001</v>
+      <c r="E22">
+        <v>56466</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>162</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="2">
-        <v>30.875</v>
+      <c r="C23">
+        <v>30875</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="2">
-        <v>35.335999999999999</v>
+      <c r="E23">
+        <v>35336</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>163</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="2">
-        <v>33.948</v>
+      <c r="C24">
+        <v>33948</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E24" s="2">
-        <v>40.691000000000003</v>
+      <c r="E24">
+        <v>40691</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>163</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="2">
-        <v>49.436</v>
+      <c r="C25">
+        <v>49436</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E25" s="2">
-        <v>58.021000000000001</v>
+      <c r="E25">
+        <v>58021</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>163</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C26" s="2">
-        <v>47.527000000000001</v>
+      <c r="C26">
+        <v>47527</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E26" s="2">
-        <v>53.296999999999997</v>
+      <c r="E26">
+        <v>53297</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>163</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C27" s="2">
-        <v>36.755000000000003</v>
+      <c r="C27">
+        <v>36755</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E27" s="2">
-        <v>43.161999999999999</v>
+      <c r="E27">
+        <v>43162</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>163</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="2">
-        <v>27.646999999999998</v>
+      <c r="C28">
+        <v>27647</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E28" s="2">
-        <v>32.552</v>
+      <c r="E28">
+        <v>32552</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>164</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="2">
-        <v>23.655999999999999</v>
+      <c r="C29">
+        <v>23656</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E29" s="2">
-        <v>27.957000000000001</v>
+      <c r="E29">
+        <v>27957</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>164</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C30" s="2">
-        <v>19.309000000000001</v>
+      <c r="C30">
+        <v>19309</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E30" s="2">
-        <v>25.062000000000001</v>
+      <c r="E30">
+        <v>25062</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>164</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="2">
-        <v>27.55</v>
+      <c r="C31">
+        <v>27550</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E31" s="2">
-        <v>32.598999999999997</v>
+      <c r="E31">
+        <v>32598.999999999996</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>164</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C32" s="2">
-        <v>25.216999999999999</v>
+      <c r="C32">
+        <v>25217</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E32" s="2">
-        <v>29.385000000000002</v>
+      <c r="E32">
+        <v>29385</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>164</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C33" s="2">
-        <v>23.132000000000001</v>
+      <c r="C33">
+        <v>23132</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E33" s="2">
-        <v>27.257999999999999</v>
+      <c r="E33">
+        <v>27258</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>165</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="2">
-        <v>22.135000000000002</v>
+      <c r="C34">
+        <v>22135</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E34" s="2">
-        <v>23.286000000000001</v>
+      <c r="E34">
+        <v>23286</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>165</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="2">
-        <v>19.193999999999999</v>
+      <c r="C35">
+        <v>19194</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E35" s="2">
-        <v>21.765999999999998</v>
+      <c r="E35">
+        <v>21766</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>165</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C36" s="2">
-        <v>23.460999999999999</v>
+      <c r="C36">
+        <v>23461</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E36" s="2">
-        <v>27.053000000000001</v>
+      <c r="E36">
+        <v>27053</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>165</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C37" s="2">
-        <v>23.416</v>
+      <c r="C37">
+        <v>23416</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E37" s="2">
-        <v>26.859000000000002</v>
+      <c r="E37">
+        <v>26859</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>165</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C38" s="2">
-        <v>19.576000000000001</v>
+      <c r="C38">
+        <v>19576</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="E38" s="2">
-        <v>20.753</v>
+      <c r="E38">
+        <v>20753</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>165</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C39" s="2">
-        <v>15.798999999999999</v>
+      <c r="C39">
+        <v>15799</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E39" s="2">
-        <v>16.408000000000001</v>
+      <c r="E39">
+        <v>16408</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>165</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C40" s="2">
-        <v>18.552</v>
+      <c r="C40">
+        <v>18552</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E40" s="2">
-        <v>21.126000000000001</v>
+      <c r="E40">
+        <v>21126</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>165</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C41" s="2">
-        <v>20.257000000000001</v>
+      <c r="C41">
+        <v>20257</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E41" s="2">
-        <v>22.12</v>
+      <c r="E41">
+        <v>22120</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>165</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C42" s="2">
-        <v>24.367000000000001</v>
+      <c r="C42">
+        <v>24367</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E42" s="2">
-        <v>27.053000000000001</v>
+      <c r="E42">
+        <v>27053</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>165</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C43" s="2">
-        <v>17.606000000000002</v>
+      <c r="C43">
+        <v>17606</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E43" s="2">
-        <v>23.526</v>
+      <c r="E43">
+        <v>23526</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>165</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C44" s="2">
-        <v>19.805</v>
+      <c r="C44">
+        <v>19805</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E44" s="2">
-        <v>23.215</v>
+      <c r="E44">
+        <v>23215</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>166</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C45" s="2">
-        <v>18.004999999999999</v>
+      <c r="C45">
+        <v>18005</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E45" s="2">
-        <v>19.709</v>
+      <c r="E45">
+        <v>19709</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>166</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C46" s="2">
-        <v>15.896000000000001</v>
+      <c r="C46">
+        <v>15896</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E46" s="2">
-        <v>18.577000000000002</v>
+      <c r="E46">
+        <v>18577</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>166</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C47" s="2">
-        <v>11.1</v>
+      <c r="C47">
+        <v>11100</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E47" s="2">
-        <v>11.67</v>
+      <c r="E47">
+        <v>11670</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>166</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C48" s="2">
-        <v>15.326000000000001</v>
+      <c r="C48">
+        <v>15326</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E48" s="2">
-        <v>17.047999999999998</v>
+      <c r="E48">
+        <v>17048</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>166</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C49" s="2">
-        <v>17.896999999999998</v>
+      <c r="C49">
+        <v>17897</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E49" s="2">
-        <v>20.728000000000002</v>
+      <c r="E49">
+        <v>20728</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>166</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C50" s="2">
-        <v>18.789000000000001</v>
+      <c r="C50">
+        <v>18789</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E50" s="2">
-        <v>21.597000000000001</v>
+      <c r="E50">
+        <v>21597</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>166</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C51" s="2">
-        <v>13.779</v>
+      <c r="C51">
+        <v>13779</v>
       </c>
       <c r="D51" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E51" s="2">
-        <v>16.02</v>
+      <c r="E51">
+        <v>16020</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>166</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C52" s="2">
-        <v>13.132</v>
+      <c r="C52">
+        <v>13132</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E52" s="2">
-        <v>15.946</v>
+      <c r="E52">
+        <v>15946</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>166</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C53" s="2">
-        <v>15.99</v>
+      <c r="C53">
+        <v>15990</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="2">
-        <v>19.157</v>
+      <c r="E53">
+        <v>19157</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>166</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C54" s="2">
-        <v>15.606999999999999</v>
+      <c r="C54">
+        <v>15607</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E54" s="2">
-        <v>16.898</v>
+      <c r="E54">
+        <v>16898</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>166</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C55" s="2">
-        <v>13.478999999999999</v>
+      <c r="C55">
+        <v>13479</v>
       </c>
       <c r="D55" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E55" s="2">
-        <v>14.688000000000001</v>
+      <c r="E55">
+        <v>14688</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>166</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C56" s="2">
-        <v>11.352</v>
+      <c r="C56">
+        <v>11352</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E56" s="2">
-        <v>11.803000000000001</v>
+      <c r="E56">
+        <v>11803</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>166</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C57" s="2">
-        <v>11.824999999999999</v>
+      <c r="C57">
+        <v>11825</v>
       </c>
       <c r="D57" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="E57" s="2">
-        <v>13.015000000000001</v>
+      <c r="E57">
+        <v>13015</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>123</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C58" s="2">
-        <v>13.73</v>
+      <c r="C58">
+        <v>13730</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E58" s="2">
-        <v>15.327</v>
+      <c r="E58">
+        <v>15327</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>123</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C59" s="2">
-        <v>14.34</v>
+      <c r="C59">
+        <v>14340</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E59" s="2">
-        <v>16.43</v>
+      <c r="E59">
+        <v>16430</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>123</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C60" s="2">
-        <v>14.375</v>
+      <c r="C60">
+        <v>14375</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="E60" s="2">
-        <v>16.971</v>
+      <c r="E60">
+        <v>16971</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>123</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C61" s="2">
-        <v>20.114000000000001</v>
+      <c r="C61">
+        <v>20114</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E61" s="2">
-        <v>23.225999999999999</v>
+      <c r="E61">
+        <v>23226</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>123</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C62" s="2">
-        <v>18.585999999999999</v>
+      <c r="C62">
+        <v>18586</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E62" s="2">
-        <v>21.452000000000002</v>
+      <c r="E62">
+        <v>21452</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>123</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C63" s="2">
-        <v>18.835999999999999</v>
+      <c r="C63">
+        <v>18836</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E63" s="2">
-        <v>21.951000000000001</v>
+      <c r="E63">
+        <v>21951</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>123</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C64" s="2">
-        <v>18.940999999999999</v>
+      <c r="C64">
+        <v>18941</v>
       </c>
       <c r="D64" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E64" s="2">
-        <v>21.952999999999999</v>
+      <c r="E64">
+        <v>21953</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>167</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C65" s="2">
-        <v>20.184000000000001</v>
+      <c r="C65">
+        <v>20184</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E65" s="2">
-        <v>23.073</v>
+      <c r="E65">
+        <v>23073</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>167</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C66" s="2">
-        <v>23.286999999999999</v>
+      <c r="C66">
+        <v>23287</v>
       </c>
       <c r="D66" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E66" s="2">
-        <v>27.536000000000001</v>
+      <c r="E66">
+        <v>27536</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>167</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C67" s="2">
-        <v>20.413</v>
+      <c r="C67">
+        <v>20413</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E67" s="2">
-        <v>25.242000000000001</v>
+      <c r="E67">
+        <v>25242</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>167</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C68" s="2">
-        <v>29.097000000000001</v>
+      <c r="C68">
+        <v>29097</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E68" s="2">
-        <v>33.588999999999999</v>
+      <c r="E68">
+        <v>33589</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>167</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="C69" s="2">
-        <v>22.004999999999999</v>
+      <c r="C69">
+        <v>22005</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="E69" s="2">
-        <v>26.24</v>
+      <c r="E69">
+        <v>26240</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>167</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C70" s="2">
-        <v>37.345999999999997</v>
+      <c r="C70">
+        <v>37346</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E70" s="2">
-        <v>43.622999999999998</v>
+      <c r="E70">
+        <v>43623</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>167</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C71" s="2">
-        <v>15.07</v>
+      <c r="C71">
+        <v>15070</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E71" s="2">
-        <v>17.722999999999999</v>
+      <c r="E71">
+        <v>17723</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>167</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C72" s="2">
-        <v>20.245999999999999</v>
+      <c r="C72">
+        <v>20246</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E72" s="2">
-        <v>24.687999999999999</v>
+      <c r="E72">
+        <v>24688</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>167</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C73" s="2">
-        <v>17.346</v>
+      <c r="C73">
+        <v>17346</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E73" s="2">
-        <v>20.404</v>
+      <c r="E73">
+        <v>20404</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>167</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C74" s="2">
-        <v>15.07</v>
+      <c r="C74">
+        <v>15070</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E74" s="2">
-        <v>14.624000000000001</v>
+      <c r="E74">
+        <v>14624</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C75" s="3">
-        <v>20.667000000000002</v>
+      <c r="C75">
+        <v>20667</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E75" s="3">
-        <v>23.215</v>
+      <c r="E75">
+        <v>23215</v>
       </c>
       <c r="F75" s="3" t="s">
         <v>80</v>

</xml_diff>